<commit_message>
renamed release files for consistency
</commit_message>
<xml_diff>
--- a/release_913-0000091_rev1_v1/913-0000091_bom.xlsx
+++ b/release_913-0000091_rev1_v1/913-0000091_bom.xlsx
@@ -115,13 +115,13 @@
     <t xml:space="preserve">Molex</t>
   </si>
   <si>
-    <t xml:space="preserve">TFC-105-02-F-D-A-K</t>
+    <t xml:space="preserve">TFC-105-02-L-D-A-K-TR</t>
   </si>
   <si>
     <t xml:space="preserve">J3</t>
   </si>
   <si>
-    <t xml:space="preserve">TFC-105-02-F-D-A-K-ND</t>
+    <t xml:space="preserve">200-TFC10502LDAKTR </t>
   </si>
   <si>
     <t xml:space="preserve">.050 X .050 TERMINAL STRIP</t>
@@ -367,7 +367,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -466,6 +466,10 @@
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -630,7 +634,7 @@
   <dimension ref="A1:IW1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.65" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1828,9 +1832,9 @@
         <v>32</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="26" t="s">
         <v>33</v>
       </c>
       <c r="H11" s="21"/>
@@ -1841,252 +1845,252 @@
       <c r="K11" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="26"/>
-      <c r="U11" s="26"/>
-      <c r="V11" s="26"/>
-      <c r="W11" s="26"/>
-      <c r="X11" s="26"/>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="26"/>
-      <c r="AA11" s="26"/>
-      <c r="AB11" s="26"/>
-      <c r="AC11" s="26"/>
-      <c r="AD11" s="26"/>
-      <c r="AE11" s="26"/>
-      <c r="AF11" s="26"/>
-      <c r="AG11" s="26"/>
-      <c r="AH11" s="26"/>
-      <c r="AI11" s="26"/>
-      <c r="AJ11" s="26"/>
-      <c r="AK11" s="26"/>
-      <c r="AL11" s="26"/>
-      <c r="AM11" s="26"/>
-      <c r="AN11" s="26"/>
-      <c r="AO11" s="26"/>
-      <c r="AP11" s="26"/>
-      <c r="AQ11" s="26"/>
-      <c r="AR11" s="26"/>
-      <c r="AS11" s="26"/>
-      <c r="AT11" s="26"/>
-      <c r="AU11" s="26"/>
-      <c r="AV11" s="26"/>
-      <c r="AW11" s="26"/>
-      <c r="AX11" s="26"/>
-      <c r="AY11" s="26"/>
-      <c r="AZ11" s="26"/>
-      <c r="BA11" s="26"/>
-      <c r="BB11" s="26"/>
-      <c r="BC11" s="26"/>
-      <c r="BD11" s="26"/>
-      <c r="BE11" s="26"/>
-      <c r="BF11" s="26"/>
-      <c r="BG11" s="26"/>
-      <c r="BH11" s="26"/>
-      <c r="BI11" s="26"/>
-      <c r="BJ11" s="26"/>
-      <c r="BK11" s="26"/>
-      <c r="BL11" s="26"/>
-      <c r="BM11" s="26"/>
-      <c r="BN11" s="26"/>
-      <c r="BO11" s="26"/>
-      <c r="BP11" s="26"/>
-      <c r="BQ11" s="26"/>
-      <c r="BR11" s="26"/>
-      <c r="BS11" s="26"/>
-      <c r="BT11" s="26"/>
-      <c r="BU11" s="26"/>
-      <c r="BV11" s="26"/>
-      <c r="BW11" s="26"/>
-      <c r="BX11" s="26"/>
-      <c r="BY11" s="26"/>
-      <c r="BZ11" s="26"/>
-      <c r="CA11" s="26"/>
-      <c r="CB11" s="26"/>
-      <c r="CC11" s="26"/>
-      <c r="CD11" s="26"/>
-      <c r="CE11" s="26"/>
-      <c r="CF11" s="26"/>
-      <c r="CG11" s="26"/>
-      <c r="CH11" s="26"/>
-      <c r="CI11" s="26"/>
-      <c r="CJ11" s="26"/>
-      <c r="CK11" s="26"/>
-      <c r="CL11" s="26"/>
-      <c r="CM11" s="26"/>
-      <c r="CN11" s="26"/>
-      <c r="CO11" s="26"/>
-      <c r="CP11" s="26"/>
-      <c r="CQ11" s="26"/>
-      <c r="CR11" s="26"/>
-      <c r="CS11" s="26"/>
-      <c r="CT11" s="26"/>
-      <c r="CU11" s="26"/>
-      <c r="CV11" s="26"/>
-      <c r="CW11" s="26"/>
-      <c r="CX11" s="26"/>
-      <c r="CY11" s="26"/>
-      <c r="CZ11" s="26"/>
-      <c r="DA11" s="26"/>
-      <c r="DB11" s="26"/>
-      <c r="DC11" s="26"/>
-      <c r="DD11" s="26"/>
-      <c r="DE11" s="26"/>
-      <c r="DF11" s="26"/>
-      <c r="DG11" s="26"/>
-      <c r="DH11" s="26"/>
-      <c r="DI11" s="26"/>
-      <c r="DJ11" s="26"/>
-      <c r="DK11" s="26"/>
-      <c r="DL11" s="26"/>
-      <c r="DM11" s="26"/>
-      <c r="DN11" s="26"/>
-      <c r="DO11" s="26"/>
-      <c r="DP11" s="26"/>
-      <c r="DQ11" s="26"/>
-      <c r="DR11" s="26"/>
-      <c r="DS11" s="26"/>
-      <c r="DT11" s="26"/>
-      <c r="DU11" s="26"/>
-      <c r="DV11" s="26"/>
-      <c r="DW11" s="26"/>
-      <c r="DX11" s="26"/>
-      <c r="DY11" s="26"/>
-      <c r="DZ11" s="26"/>
-      <c r="EA11" s="26"/>
-      <c r="EB11" s="26"/>
-      <c r="EC11" s="26"/>
-      <c r="ED11" s="26"/>
-      <c r="EE11" s="26"/>
-      <c r="EF11" s="26"/>
-      <c r="EG11" s="26"/>
-      <c r="EH11" s="26"/>
-      <c r="EI11" s="26"/>
-      <c r="EJ11" s="26"/>
-      <c r="EK11" s="26"/>
-      <c r="EL11" s="26"/>
-      <c r="EM11" s="26"/>
-      <c r="EN11" s="26"/>
-      <c r="EO11" s="26"/>
-      <c r="EP11" s="26"/>
-      <c r="EQ11" s="26"/>
-      <c r="ER11" s="26"/>
-      <c r="ES11" s="26"/>
-      <c r="ET11" s="26"/>
-      <c r="EU11" s="26"/>
-      <c r="EV11" s="26"/>
-      <c r="EW11" s="26"/>
-      <c r="EX11" s="26"/>
-      <c r="EY11" s="26"/>
-      <c r="EZ11" s="26"/>
-      <c r="FA11" s="26"/>
-      <c r="FB11" s="26"/>
-      <c r="FC11" s="26"/>
-      <c r="FD11" s="26"/>
-      <c r="FE11" s="26"/>
-      <c r="FF11" s="26"/>
-      <c r="FG11" s="26"/>
-      <c r="FH11" s="26"/>
-      <c r="FI11" s="26"/>
-      <c r="FJ11" s="26"/>
-      <c r="FK11" s="26"/>
-      <c r="FL11" s="26"/>
-      <c r="FM11" s="26"/>
-      <c r="FN11" s="26"/>
-      <c r="FO11" s="26"/>
-      <c r="FP11" s="26"/>
-      <c r="FQ11" s="26"/>
-      <c r="FR11" s="26"/>
-      <c r="FS11" s="26"/>
-      <c r="FT11" s="26"/>
-      <c r="FU11" s="26"/>
-      <c r="FV11" s="26"/>
-      <c r="FW11" s="26"/>
-      <c r="FX11" s="26"/>
-      <c r="FY11" s="26"/>
-      <c r="FZ11" s="26"/>
-      <c r="GA11" s="26"/>
-      <c r="GB11" s="26"/>
-      <c r="GC11" s="26"/>
-      <c r="GD11" s="26"/>
-      <c r="GE11" s="26"/>
-      <c r="GF11" s="26"/>
-      <c r="GG11" s="26"/>
-      <c r="GH11" s="26"/>
-      <c r="GI11" s="26"/>
-      <c r="GJ11" s="26"/>
-      <c r="GK11" s="26"/>
-      <c r="GL11" s="26"/>
-      <c r="GM11" s="26"/>
-      <c r="GN11" s="26"/>
-      <c r="GO11" s="26"/>
-      <c r="GP11" s="26"/>
-      <c r="GQ11" s="26"/>
-      <c r="GR11" s="26"/>
-      <c r="GS11" s="26"/>
-      <c r="GT11" s="26"/>
-      <c r="GU11" s="26"/>
-      <c r="GV11" s="26"/>
-      <c r="GW11" s="26"/>
-      <c r="GX11" s="26"/>
-      <c r="GY11" s="26"/>
-      <c r="GZ11" s="26"/>
-      <c r="HA11" s="26"/>
-      <c r="HB11" s="26"/>
-      <c r="HC11" s="26"/>
-      <c r="HD11" s="26"/>
-      <c r="HE11" s="26"/>
-      <c r="HF11" s="26"/>
-      <c r="HG11" s="26"/>
-      <c r="HH11" s="26"/>
-      <c r="HI11" s="26"/>
-      <c r="HJ11" s="26"/>
-      <c r="HK11" s="26"/>
-      <c r="HL11" s="26"/>
-      <c r="HM11" s="26"/>
-      <c r="HN11" s="26"/>
-      <c r="HO11" s="26"/>
-      <c r="HP11" s="26"/>
-      <c r="HQ11" s="26"/>
-      <c r="HR11" s="26"/>
-      <c r="HS11" s="26"/>
-      <c r="HT11" s="26"/>
-      <c r="HU11" s="26"/>
-      <c r="HV11" s="26"/>
-      <c r="HW11" s="26"/>
-      <c r="HX11" s="26"/>
-      <c r="HY11" s="26"/>
-      <c r="HZ11" s="26"/>
-      <c r="IA11" s="26"/>
-      <c r="IB11" s="26"/>
-      <c r="IC11" s="26"/>
-      <c r="ID11" s="26"/>
-      <c r="IE11" s="26"/>
-      <c r="IF11" s="26"/>
-      <c r="IG11" s="26"/>
-      <c r="IH11" s="26"/>
-      <c r="II11" s="26"/>
-      <c r="IJ11" s="26"/>
-      <c r="IK11" s="26"/>
-      <c r="IL11" s="26"/>
-      <c r="IM11" s="26"/>
-      <c r="IN11" s="26"/>
-      <c r="IO11" s="26"/>
-      <c r="IP11" s="26"/>
-      <c r="IQ11" s="26"/>
-      <c r="IR11" s="26"/>
-      <c r="IS11" s="26"/>
-      <c r="IT11" s="26"/>
-      <c r="IU11" s="26"/>
-      <c r="IV11" s="26"/>
-      <c r="IW11" s="26"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="27"/>
+      <c r="AA11" s="27"/>
+      <c r="AB11" s="27"/>
+      <c r="AC11" s="27"/>
+      <c r="AD11" s="27"/>
+      <c r="AE11" s="27"/>
+      <c r="AF11" s="27"/>
+      <c r="AG11" s="27"/>
+      <c r="AH11" s="27"/>
+      <c r="AI11" s="27"/>
+      <c r="AJ11" s="27"/>
+      <c r="AK11" s="27"/>
+      <c r="AL11" s="27"/>
+      <c r="AM11" s="27"/>
+      <c r="AN11" s="27"/>
+      <c r="AO11" s="27"/>
+      <c r="AP11" s="27"/>
+      <c r="AQ11" s="27"/>
+      <c r="AR11" s="27"/>
+      <c r="AS11" s="27"/>
+      <c r="AT11" s="27"/>
+      <c r="AU11" s="27"/>
+      <c r="AV11" s="27"/>
+      <c r="AW11" s="27"/>
+      <c r="AX11" s="27"/>
+      <c r="AY11" s="27"/>
+      <c r="AZ11" s="27"/>
+      <c r="BA11" s="27"/>
+      <c r="BB11" s="27"/>
+      <c r="BC11" s="27"/>
+      <c r="BD11" s="27"/>
+      <c r="BE11" s="27"/>
+      <c r="BF11" s="27"/>
+      <c r="BG11" s="27"/>
+      <c r="BH11" s="27"/>
+      <c r="BI11" s="27"/>
+      <c r="BJ11" s="27"/>
+      <c r="BK11" s="27"/>
+      <c r="BL11" s="27"/>
+      <c r="BM11" s="27"/>
+      <c r="BN11" s="27"/>
+      <c r="BO11" s="27"/>
+      <c r="BP11" s="27"/>
+      <c r="BQ11" s="27"/>
+      <c r="BR11" s="27"/>
+      <c r="BS11" s="27"/>
+      <c r="BT11" s="27"/>
+      <c r="BU11" s="27"/>
+      <c r="BV11" s="27"/>
+      <c r="BW11" s="27"/>
+      <c r="BX11" s="27"/>
+      <c r="BY11" s="27"/>
+      <c r="BZ11" s="27"/>
+      <c r="CA11" s="27"/>
+      <c r="CB11" s="27"/>
+      <c r="CC11" s="27"/>
+      <c r="CD11" s="27"/>
+      <c r="CE11" s="27"/>
+      <c r="CF11" s="27"/>
+      <c r="CG11" s="27"/>
+      <c r="CH11" s="27"/>
+      <c r="CI11" s="27"/>
+      <c r="CJ11" s="27"/>
+      <c r="CK11" s="27"/>
+      <c r="CL11" s="27"/>
+      <c r="CM11" s="27"/>
+      <c r="CN11" s="27"/>
+      <c r="CO11" s="27"/>
+      <c r="CP11" s="27"/>
+      <c r="CQ11" s="27"/>
+      <c r="CR11" s="27"/>
+      <c r="CS11" s="27"/>
+      <c r="CT11" s="27"/>
+      <c r="CU11" s="27"/>
+      <c r="CV11" s="27"/>
+      <c r="CW11" s="27"/>
+      <c r="CX11" s="27"/>
+      <c r="CY11" s="27"/>
+      <c r="CZ11" s="27"/>
+      <c r="DA11" s="27"/>
+      <c r="DB11" s="27"/>
+      <c r="DC11" s="27"/>
+      <c r="DD11" s="27"/>
+      <c r="DE11" s="27"/>
+      <c r="DF11" s="27"/>
+      <c r="DG11" s="27"/>
+      <c r="DH11" s="27"/>
+      <c r="DI11" s="27"/>
+      <c r="DJ11" s="27"/>
+      <c r="DK11" s="27"/>
+      <c r="DL11" s="27"/>
+      <c r="DM11" s="27"/>
+      <c r="DN11" s="27"/>
+      <c r="DO11" s="27"/>
+      <c r="DP11" s="27"/>
+      <c r="DQ11" s="27"/>
+      <c r="DR11" s="27"/>
+      <c r="DS11" s="27"/>
+      <c r="DT11" s="27"/>
+      <c r="DU11" s="27"/>
+      <c r="DV11" s="27"/>
+      <c r="DW11" s="27"/>
+      <c r="DX11" s="27"/>
+      <c r="DY11" s="27"/>
+      <c r="DZ11" s="27"/>
+      <c r="EA11" s="27"/>
+      <c r="EB11" s="27"/>
+      <c r="EC11" s="27"/>
+      <c r="ED11" s="27"/>
+      <c r="EE11" s="27"/>
+      <c r="EF11" s="27"/>
+      <c r="EG11" s="27"/>
+      <c r="EH11" s="27"/>
+      <c r="EI11" s="27"/>
+      <c r="EJ11" s="27"/>
+      <c r="EK11" s="27"/>
+      <c r="EL11" s="27"/>
+      <c r="EM11" s="27"/>
+      <c r="EN11" s="27"/>
+      <c r="EO11" s="27"/>
+      <c r="EP11" s="27"/>
+      <c r="EQ11" s="27"/>
+      <c r="ER11" s="27"/>
+      <c r="ES11" s="27"/>
+      <c r="ET11" s="27"/>
+      <c r="EU11" s="27"/>
+      <c r="EV11" s="27"/>
+      <c r="EW11" s="27"/>
+      <c r="EX11" s="27"/>
+      <c r="EY11" s="27"/>
+      <c r="EZ11" s="27"/>
+      <c r="FA11" s="27"/>
+      <c r="FB11" s="27"/>
+      <c r="FC11" s="27"/>
+      <c r="FD11" s="27"/>
+      <c r="FE11" s="27"/>
+      <c r="FF11" s="27"/>
+      <c r="FG11" s="27"/>
+      <c r="FH11" s="27"/>
+      <c r="FI11" s="27"/>
+      <c r="FJ11" s="27"/>
+      <c r="FK11" s="27"/>
+      <c r="FL11" s="27"/>
+      <c r="FM11" s="27"/>
+      <c r="FN11" s="27"/>
+      <c r="FO11" s="27"/>
+      <c r="FP11" s="27"/>
+      <c r="FQ11" s="27"/>
+      <c r="FR11" s="27"/>
+      <c r="FS11" s="27"/>
+      <c r="FT11" s="27"/>
+      <c r="FU11" s="27"/>
+      <c r="FV11" s="27"/>
+      <c r="FW11" s="27"/>
+      <c r="FX11" s="27"/>
+      <c r="FY11" s="27"/>
+      <c r="FZ11" s="27"/>
+      <c r="GA11" s="27"/>
+      <c r="GB11" s="27"/>
+      <c r="GC11" s="27"/>
+      <c r="GD11" s="27"/>
+      <c r="GE11" s="27"/>
+      <c r="GF11" s="27"/>
+      <c r="GG11" s="27"/>
+      <c r="GH11" s="27"/>
+      <c r="GI11" s="27"/>
+      <c r="GJ11" s="27"/>
+      <c r="GK11" s="27"/>
+      <c r="GL11" s="27"/>
+      <c r="GM11" s="27"/>
+      <c r="GN11" s="27"/>
+      <c r="GO11" s="27"/>
+      <c r="GP11" s="27"/>
+      <c r="GQ11" s="27"/>
+      <c r="GR11" s="27"/>
+      <c r="GS11" s="27"/>
+      <c r="GT11" s="27"/>
+      <c r="GU11" s="27"/>
+      <c r="GV11" s="27"/>
+      <c r="GW11" s="27"/>
+      <c r="GX11" s="27"/>
+      <c r="GY11" s="27"/>
+      <c r="GZ11" s="27"/>
+      <c r="HA11" s="27"/>
+      <c r="HB11" s="27"/>
+      <c r="HC11" s="27"/>
+      <c r="HD11" s="27"/>
+      <c r="HE11" s="27"/>
+      <c r="HF11" s="27"/>
+      <c r="HG11" s="27"/>
+      <c r="HH11" s="27"/>
+      <c r="HI11" s="27"/>
+      <c r="HJ11" s="27"/>
+      <c r="HK11" s="27"/>
+      <c r="HL11" s="27"/>
+      <c r="HM11" s="27"/>
+      <c r="HN11" s="27"/>
+      <c r="HO11" s="27"/>
+      <c r="HP11" s="27"/>
+      <c r="HQ11" s="27"/>
+      <c r="HR11" s="27"/>
+      <c r="HS11" s="27"/>
+      <c r="HT11" s="27"/>
+      <c r="HU11" s="27"/>
+      <c r="HV11" s="27"/>
+      <c r="HW11" s="27"/>
+      <c r="HX11" s="27"/>
+      <c r="HY11" s="27"/>
+      <c r="HZ11" s="27"/>
+      <c r="IA11" s="27"/>
+      <c r="IB11" s="27"/>
+      <c r="IC11" s="27"/>
+      <c r="ID11" s="27"/>
+      <c r="IE11" s="27"/>
+      <c r="IF11" s="27"/>
+      <c r="IG11" s="27"/>
+      <c r="IH11" s="27"/>
+      <c r="II11" s="27"/>
+      <c r="IJ11" s="27"/>
+      <c r="IK11" s="27"/>
+      <c r="IL11" s="27"/>
+      <c r="IM11" s="27"/>
+      <c r="IN11" s="27"/>
+      <c r="IO11" s="27"/>
+      <c r="IP11" s="27"/>
+      <c r="IQ11" s="27"/>
+      <c r="IR11" s="27"/>
+      <c r="IS11" s="27"/>
+      <c r="IT11" s="27"/>
+      <c r="IU11" s="27"/>
+      <c r="IV11" s="27"/>
+      <c r="IW11" s="27"/>
     </row>
     <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="21" t="n">
@@ -2118,252 +2122,252 @@
       <c r="K12" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
-      <c r="U12" s="26"/>
-      <c r="V12" s="26"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="26"/>
-      <c r="Y12" s="26"/>
-      <c r="Z12" s="26"/>
-      <c r="AA12" s="26"/>
-      <c r="AB12" s="26"/>
-      <c r="AC12" s="26"/>
-      <c r="AD12" s="26"/>
-      <c r="AE12" s="26"/>
-      <c r="AF12" s="26"/>
-      <c r="AG12" s="26"/>
-      <c r="AH12" s="26"/>
-      <c r="AI12" s="26"/>
-      <c r="AJ12" s="26"/>
-      <c r="AK12" s="26"/>
-      <c r="AL12" s="26"/>
-      <c r="AM12" s="26"/>
-      <c r="AN12" s="26"/>
-      <c r="AO12" s="26"/>
-      <c r="AP12" s="26"/>
-      <c r="AQ12" s="26"/>
-      <c r="AR12" s="26"/>
-      <c r="AS12" s="26"/>
-      <c r="AT12" s="26"/>
-      <c r="AU12" s="26"/>
-      <c r="AV12" s="26"/>
-      <c r="AW12" s="26"/>
-      <c r="AX12" s="26"/>
-      <c r="AY12" s="26"/>
-      <c r="AZ12" s="26"/>
-      <c r="BA12" s="26"/>
-      <c r="BB12" s="26"/>
-      <c r="BC12" s="26"/>
-      <c r="BD12" s="26"/>
-      <c r="BE12" s="26"/>
-      <c r="BF12" s="26"/>
-      <c r="BG12" s="26"/>
-      <c r="BH12" s="26"/>
-      <c r="BI12" s="26"/>
-      <c r="BJ12" s="26"/>
-      <c r="BK12" s="26"/>
-      <c r="BL12" s="26"/>
-      <c r="BM12" s="26"/>
-      <c r="BN12" s="26"/>
-      <c r="BO12" s="26"/>
-      <c r="BP12" s="26"/>
-      <c r="BQ12" s="26"/>
-      <c r="BR12" s="26"/>
-      <c r="BS12" s="26"/>
-      <c r="BT12" s="26"/>
-      <c r="BU12" s="26"/>
-      <c r="BV12" s="26"/>
-      <c r="BW12" s="26"/>
-      <c r="BX12" s="26"/>
-      <c r="BY12" s="26"/>
-      <c r="BZ12" s="26"/>
-      <c r="CA12" s="26"/>
-      <c r="CB12" s="26"/>
-      <c r="CC12" s="26"/>
-      <c r="CD12" s="26"/>
-      <c r="CE12" s="26"/>
-      <c r="CF12" s="26"/>
-      <c r="CG12" s="26"/>
-      <c r="CH12" s="26"/>
-      <c r="CI12" s="26"/>
-      <c r="CJ12" s="26"/>
-      <c r="CK12" s="26"/>
-      <c r="CL12" s="26"/>
-      <c r="CM12" s="26"/>
-      <c r="CN12" s="26"/>
-      <c r="CO12" s="26"/>
-      <c r="CP12" s="26"/>
-      <c r="CQ12" s="26"/>
-      <c r="CR12" s="26"/>
-      <c r="CS12" s="26"/>
-      <c r="CT12" s="26"/>
-      <c r="CU12" s="26"/>
-      <c r="CV12" s="26"/>
-      <c r="CW12" s="26"/>
-      <c r="CX12" s="26"/>
-      <c r="CY12" s="26"/>
-      <c r="CZ12" s="26"/>
-      <c r="DA12" s="26"/>
-      <c r="DB12" s="26"/>
-      <c r="DC12" s="26"/>
-      <c r="DD12" s="26"/>
-      <c r="DE12" s="26"/>
-      <c r="DF12" s="26"/>
-      <c r="DG12" s="26"/>
-      <c r="DH12" s="26"/>
-      <c r="DI12" s="26"/>
-      <c r="DJ12" s="26"/>
-      <c r="DK12" s="26"/>
-      <c r="DL12" s="26"/>
-      <c r="DM12" s="26"/>
-      <c r="DN12" s="26"/>
-      <c r="DO12" s="26"/>
-      <c r="DP12" s="26"/>
-      <c r="DQ12" s="26"/>
-      <c r="DR12" s="26"/>
-      <c r="DS12" s="26"/>
-      <c r="DT12" s="26"/>
-      <c r="DU12" s="26"/>
-      <c r="DV12" s="26"/>
-      <c r="DW12" s="26"/>
-      <c r="DX12" s="26"/>
-      <c r="DY12" s="26"/>
-      <c r="DZ12" s="26"/>
-      <c r="EA12" s="26"/>
-      <c r="EB12" s="26"/>
-      <c r="EC12" s="26"/>
-      <c r="ED12" s="26"/>
-      <c r="EE12" s="26"/>
-      <c r="EF12" s="26"/>
-      <c r="EG12" s="26"/>
-      <c r="EH12" s="26"/>
-      <c r="EI12" s="26"/>
-      <c r="EJ12" s="26"/>
-      <c r="EK12" s="26"/>
-      <c r="EL12" s="26"/>
-      <c r="EM12" s="26"/>
-      <c r="EN12" s="26"/>
-      <c r="EO12" s="26"/>
-      <c r="EP12" s="26"/>
-      <c r="EQ12" s="26"/>
-      <c r="ER12" s="26"/>
-      <c r="ES12" s="26"/>
-      <c r="ET12" s="26"/>
-      <c r="EU12" s="26"/>
-      <c r="EV12" s="26"/>
-      <c r="EW12" s="26"/>
-      <c r="EX12" s="26"/>
-      <c r="EY12" s="26"/>
-      <c r="EZ12" s="26"/>
-      <c r="FA12" s="26"/>
-      <c r="FB12" s="26"/>
-      <c r="FC12" s="26"/>
-      <c r="FD12" s="26"/>
-      <c r="FE12" s="26"/>
-      <c r="FF12" s="26"/>
-      <c r="FG12" s="26"/>
-      <c r="FH12" s="26"/>
-      <c r="FI12" s="26"/>
-      <c r="FJ12" s="26"/>
-      <c r="FK12" s="26"/>
-      <c r="FL12" s="26"/>
-      <c r="FM12" s="26"/>
-      <c r="FN12" s="26"/>
-      <c r="FO12" s="26"/>
-      <c r="FP12" s="26"/>
-      <c r="FQ12" s="26"/>
-      <c r="FR12" s="26"/>
-      <c r="FS12" s="26"/>
-      <c r="FT12" s="26"/>
-      <c r="FU12" s="26"/>
-      <c r="FV12" s="26"/>
-      <c r="FW12" s="26"/>
-      <c r="FX12" s="26"/>
-      <c r="FY12" s="26"/>
-      <c r="FZ12" s="26"/>
-      <c r="GA12" s="26"/>
-      <c r="GB12" s="26"/>
-      <c r="GC12" s="26"/>
-      <c r="GD12" s="26"/>
-      <c r="GE12" s="26"/>
-      <c r="GF12" s="26"/>
-      <c r="GG12" s="26"/>
-      <c r="GH12" s="26"/>
-      <c r="GI12" s="26"/>
-      <c r="GJ12" s="26"/>
-      <c r="GK12" s="26"/>
-      <c r="GL12" s="26"/>
-      <c r="GM12" s="26"/>
-      <c r="GN12" s="26"/>
-      <c r="GO12" s="26"/>
-      <c r="GP12" s="26"/>
-      <c r="GQ12" s="26"/>
-      <c r="GR12" s="26"/>
-      <c r="GS12" s="26"/>
-      <c r="GT12" s="26"/>
-      <c r="GU12" s="26"/>
-      <c r="GV12" s="26"/>
-      <c r="GW12" s="26"/>
-      <c r="GX12" s="26"/>
-      <c r="GY12" s="26"/>
-      <c r="GZ12" s="26"/>
-      <c r="HA12" s="26"/>
-      <c r="HB12" s="26"/>
-      <c r="HC12" s="26"/>
-      <c r="HD12" s="26"/>
-      <c r="HE12" s="26"/>
-      <c r="HF12" s="26"/>
-      <c r="HG12" s="26"/>
-      <c r="HH12" s="26"/>
-      <c r="HI12" s="26"/>
-      <c r="HJ12" s="26"/>
-      <c r="HK12" s="26"/>
-      <c r="HL12" s="26"/>
-      <c r="HM12" s="26"/>
-      <c r="HN12" s="26"/>
-      <c r="HO12" s="26"/>
-      <c r="HP12" s="26"/>
-      <c r="HQ12" s="26"/>
-      <c r="HR12" s="26"/>
-      <c r="HS12" s="26"/>
-      <c r="HT12" s="26"/>
-      <c r="HU12" s="26"/>
-      <c r="HV12" s="26"/>
-      <c r="HW12" s="26"/>
-      <c r="HX12" s="26"/>
-      <c r="HY12" s="26"/>
-      <c r="HZ12" s="26"/>
-      <c r="IA12" s="26"/>
-      <c r="IB12" s="26"/>
-      <c r="IC12" s="26"/>
-      <c r="ID12" s="26"/>
-      <c r="IE12" s="26"/>
-      <c r="IF12" s="26"/>
-      <c r="IG12" s="26"/>
-      <c r="IH12" s="26"/>
-      <c r="II12" s="26"/>
-      <c r="IJ12" s="26"/>
-      <c r="IK12" s="26"/>
-      <c r="IL12" s="26"/>
-      <c r="IM12" s="26"/>
-      <c r="IN12" s="26"/>
-      <c r="IO12" s="26"/>
-      <c r="IP12" s="26"/>
-      <c r="IQ12" s="26"/>
-      <c r="IR12" s="26"/>
-      <c r="IS12" s="26"/>
-      <c r="IT12" s="26"/>
-      <c r="IU12" s="26"/>
-      <c r="IV12" s="26"/>
-      <c r="IW12" s="26"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="27"/>
+      <c r="AA12" s="27"/>
+      <c r="AB12" s="27"/>
+      <c r="AC12" s="27"/>
+      <c r="AD12" s="27"/>
+      <c r="AE12" s="27"/>
+      <c r="AF12" s="27"/>
+      <c r="AG12" s="27"/>
+      <c r="AH12" s="27"/>
+      <c r="AI12" s="27"/>
+      <c r="AJ12" s="27"/>
+      <c r="AK12" s="27"/>
+      <c r="AL12" s="27"/>
+      <c r="AM12" s="27"/>
+      <c r="AN12" s="27"/>
+      <c r="AO12" s="27"/>
+      <c r="AP12" s="27"/>
+      <c r="AQ12" s="27"/>
+      <c r="AR12" s="27"/>
+      <c r="AS12" s="27"/>
+      <c r="AT12" s="27"/>
+      <c r="AU12" s="27"/>
+      <c r="AV12" s="27"/>
+      <c r="AW12" s="27"/>
+      <c r="AX12" s="27"/>
+      <c r="AY12" s="27"/>
+      <c r="AZ12" s="27"/>
+      <c r="BA12" s="27"/>
+      <c r="BB12" s="27"/>
+      <c r="BC12" s="27"/>
+      <c r="BD12" s="27"/>
+      <c r="BE12" s="27"/>
+      <c r="BF12" s="27"/>
+      <c r="BG12" s="27"/>
+      <c r="BH12" s="27"/>
+      <c r="BI12" s="27"/>
+      <c r="BJ12" s="27"/>
+      <c r="BK12" s="27"/>
+      <c r="BL12" s="27"/>
+      <c r="BM12" s="27"/>
+      <c r="BN12" s="27"/>
+      <c r="BO12" s="27"/>
+      <c r="BP12" s="27"/>
+      <c r="BQ12" s="27"/>
+      <c r="BR12" s="27"/>
+      <c r="BS12" s="27"/>
+      <c r="BT12" s="27"/>
+      <c r="BU12" s="27"/>
+      <c r="BV12" s="27"/>
+      <c r="BW12" s="27"/>
+      <c r="BX12" s="27"/>
+      <c r="BY12" s="27"/>
+      <c r="BZ12" s="27"/>
+      <c r="CA12" s="27"/>
+      <c r="CB12" s="27"/>
+      <c r="CC12" s="27"/>
+      <c r="CD12" s="27"/>
+      <c r="CE12" s="27"/>
+      <c r="CF12" s="27"/>
+      <c r="CG12" s="27"/>
+      <c r="CH12" s="27"/>
+      <c r="CI12" s="27"/>
+      <c r="CJ12" s="27"/>
+      <c r="CK12" s="27"/>
+      <c r="CL12" s="27"/>
+      <c r="CM12" s="27"/>
+      <c r="CN12" s="27"/>
+      <c r="CO12" s="27"/>
+      <c r="CP12" s="27"/>
+      <c r="CQ12" s="27"/>
+      <c r="CR12" s="27"/>
+      <c r="CS12" s="27"/>
+      <c r="CT12" s="27"/>
+      <c r="CU12" s="27"/>
+      <c r="CV12" s="27"/>
+      <c r="CW12" s="27"/>
+      <c r="CX12" s="27"/>
+      <c r="CY12" s="27"/>
+      <c r="CZ12" s="27"/>
+      <c r="DA12" s="27"/>
+      <c r="DB12" s="27"/>
+      <c r="DC12" s="27"/>
+      <c r="DD12" s="27"/>
+      <c r="DE12" s="27"/>
+      <c r="DF12" s="27"/>
+      <c r="DG12" s="27"/>
+      <c r="DH12" s="27"/>
+      <c r="DI12" s="27"/>
+      <c r="DJ12" s="27"/>
+      <c r="DK12" s="27"/>
+      <c r="DL12" s="27"/>
+      <c r="DM12" s="27"/>
+      <c r="DN12" s="27"/>
+      <c r="DO12" s="27"/>
+      <c r="DP12" s="27"/>
+      <c r="DQ12" s="27"/>
+      <c r="DR12" s="27"/>
+      <c r="DS12" s="27"/>
+      <c r="DT12" s="27"/>
+      <c r="DU12" s="27"/>
+      <c r="DV12" s="27"/>
+      <c r="DW12" s="27"/>
+      <c r="DX12" s="27"/>
+      <c r="DY12" s="27"/>
+      <c r="DZ12" s="27"/>
+      <c r="EA12" s="27"/>
+      <c r="EB12" s="27"/>
+      <c r="EC12" s="27"/>
+      <c r="ED12" s="27"/>
+      <c r="EE12" s="27"/>
+      <c r="EF12" s="27"/>
+      <c r="EG12" s="27"/>
+      <c r="EH12" s="27"/>
+      <c r="EI12" s="27"/>
+      <c r="EJ12" s="27"/>
+      <c r="EK12" s="27"/>
+      <c r="EL12" s="27"/>
+      <c r="EM12" s="27"/>
+      <c r="EN12" s="27"/>
+      <c r="EO12" s="27"/>
+      <c r="EP12" s="27"/>
+      <c r="EQ12" s="27"/>
+      <c r="ER12" s="27"/>
+      <c r="ES12" s="27"/>
+      <c r="ET12" s="27"/>
+      <c r="EU12" s="27"/>
+      <c r="EV12" s="27"/>
+      <c r="EW12" s="27"/>
+      <c r="EX12" s="27"/>
+      <c r="EY12" s="27"/>
+      <c r="EZ12" s="27"/>
+      <c r="FA12" s="27"/>
+      <c r="FB12" s="27"/>
+      <c r="FC12" s="27"/>
+      <c r="FD12" s="27"/>
+      <c r="FE12" s="27"/>
+      <c r="FF12" s="27"/>
+      <c r="FG12" s="27"/>
+      <c r="FH12" s="27"/>
+      <c r="FI12" s="27"/>
+      <c r="FJ12" s="27"/>
+      <c r="FK12" s="27"/>
+      <c r="FL12" s="27"/>
+      <c r="FM12" s="27"/>
+      <c r="FN12" s="27"/>
+      <c r="FO12" s="27"/>
+      <c r="FP12" s="27"/>
+      <c r="FQ12" s="27"/>
+      <c r="FR12" s="27"/>
+      <c r="FS12" s="27"/>
+      <c r="FT12" s="27"/>
+      <c r="FU12" s="27"/>
+      <c r="FV12" s="27"/>
+      <c r="FW12" s="27"/>
+      <c r="FX12" s="27"/>
+      <c r="FY12" s="27"/>
+      <c r="FZ12" s="27"/>
+      <c r="GA12" s="27"/>
+      <c r="GB12" s="27"/>
+      <c r="GC12" s="27"/>
+      <c r="GD12" s="27"/>
+      <c r="GE12" s="27"/>
+      <c r="GF12" s="27"/>
+      <c r="GG12" s="27"/>
+      <c r="GH12" s="27"/>
+      <c r="GI12" s="27"/>
+      <c r="GJ12" s="27"/>
+      <c r="GK12" s="27"/>
+      <c r="GL12" s="27"/>
+      <c r="GM12" s="27"/>
+      <c r="GN12" s="27"/>
+      <c r="GO12" s="27"/>
+      <c r="GP12" s="27"/>
+      <c r="GQ12" s="27"/>
+      <c r="GR12" s="27"/>
+      <c r="GS12" s="27"/>
+      <c r="GT12" s="27"/>
+      <c r="GU12" s="27"/>
+      <c r="GV12" s="27"/>
+      <c r="GW12" s="27"/>
+      <c r="GX12" s="27"/>
+      <c r="GY12" s="27"/>
+      <c r="GZ12" s="27"/>
+      <c r="HA12" s="27"/>
+      <c r="HB12" s="27"/>
+      <c r="HC12" s="27"/>
+      <c r="HD12" s="27"/>
+      <c r="HE12" s="27"/>
+      <c r="HF12" s="27"/>
+      <c r="HG12" s="27"/>
+      <c r="HH12" s="27"/>
+      <c r="HI12" s="27"/>
+      <c r="HJ12" s="27"/>
+      <c r="HK12" s="27"/>
+      <c r="HL12" s="27"/>
+      <c r="HM12" s="27"/>
+      <c r="HN12" s="27"/>
+      <c r="HO12" s="27"/>
+      <c r="HP12" s="27"/>
+      <c r="HQ12" s="27"/>
+      <c r="HR12" s="27"/>
+      <c r="HS12" s="27"/>
+      <c r="HT12" s="27"/>
+      <c r="HU12" s="27"/>
+      <c r="HV12" s="27"/>
+      <c r="HW12" s="27"/>
+      <c r="HX12" s="27"/>
+      <c r="HY12" s="27"/>
+      <c r="HZ12" s="27"/>
+      <c r="IA12" s="27"/>
+      <c r="IB12" s="27"/>
+      <c r="IC12" s="27"/>
+      <c r="ID12" s="27"/>
+      <c r="IE12" s="27"/>
+      <c r="IF12" s="27"/>
+      <c r="IG12" s="27"/>
+      <c r="IH12" s="27"/>
+      <c r="II12" s="27"/>
+      <c r="IJ12" s="27"/>
+      <c r="IK12" s="27"/>
+      <c r="IL12" s="27"/>
+      <c r="IM12" s="27"/>
+      <c r="IN12" s="27"/>
+      <c r="IO12" s="27"/>
+      <c r="IP12" s="27"/>
+      <c r="IQ12" s="27"/>
+      <c r="IR12" s="27"/>
+      <c r="IS12" s="27"/>
+      <c r="IT12" s="27"/>
+      <c r="IU12" s="27"/>
+      <c r="IV12" s="27"/>
+      <c r="IW12" s="27"/>
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="21" t="n">
@@ -2395,252 +2399,252 @@
       <c r="K13" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="26"/>
-      <c r="T13" s="26"/>
-      <c r="U13" s="26"/>
-      <c r="V13" s="26"/>
-      <c r="W13" s="26"/>
-      <c r="X13" s="26"/>
-      <c r="Y13" s="26"/>
-      <c r="Z13" s="26"/>
-      <c r="AA13" s="26"/>
-      <c r="AB13" s="26"/>
-      <c r="AC13" s="26"/>
-      <c r="AD13" s="26"/>
-      <c r="AE13" s="26"/>
-      <c r="AF13" s="26"/>
-      <c r="AG13" s="26"/>
-      <c r="AH13" s="26"/>
-      <c r="AI13" s="26"/>
-      <c r="AJ13" s="26"/>
-      <c r="AK13" s="26"/>
-      <c r="AL13" s="26"/>
-      <c r="AM13" s="26"/>
-      <c r="AN13" s="26"/>
-      <c r="AO13" s="26"/>
-      <c r="AP13" s="26"/>
-      <c r="AQ13" s="26"/>
-      <c r="AR13" s="26"/>
-      <c r="AS13" s="26"/>
-      <c r="AT13" s="26"/>
-      <c r="AU13" s="26"/>
-      <c r="AV13" s="26"/>
-      <c r="AW13" s="26"/>
-      <c r="AX13" s="26"/>
-      <c r="AY13" s="26"/>
-      <c r="AZ13" s="26"/>
-      <c r="BA13" s="26"/>
-      <c r="BB13" s="26"/>
-      <c r="BC13" s="26"/>
-      <c r="BD13" s="26"/>
-      <c r="BE13" s="26"/>
-      <c r="BF13" s="26"/>
-      <c r="BG13" s="26"/>
-      <c r="BH13" s="26"/>
-      <c r="BI13" s="26"/>
-      <c r="BJ13" s="26"/>
-      <c r="BK13" s="26"/>
-      <c r="BL13" s="26"/>
-      <c r="BM13" s="26"/>
-      <c r="BN13" s="26"/>
-      <c r="BO13" s="26"/>
-      <c r="BP13" s="26"/>
-      <c r="BQ13" s="26"/>
-      <c r="BR13" s="26"/>
-      <c r="BS13" s="26"/>
-      <c r="BT13" s="26"/>
-      <c r="BU13" s="26"/>
-      <c r="BV13" s="26"/>
-      <c r="BW13" s="26"/>
-      <c r="BX13" s="26"/>
-      <c r="BY13" s="26"/>
-      <c r="BZ13" s="26"/>
-      <c r="CA13" s="26"/>
-      <c r="CB13" s="26"/>
-      <c r="CC13" s="26"/>
-      <c r="CD13" s="26"/>
-      <c r="CE13" s="26"/>
-      <c r="CF13" s="26"/>
-      <c r="CG13" s="26"/>
-      <c r="CH13" s="26"/>
-      <c r="CI13" s="26"/>
-      <c r="CJ13" s="26"/>
-      <c r="CK13" s="26"/>
-      <c r="CL13" s="26"/>
-      <c r="CM13" s="26"/>
-      <c r="CN13" s="26"/>
-      <c r="CO13" s="26"/>
-      <c r="CP13" s="26"/>
-      <c r="CQ13" s="26"/>
-      <c r="CR13" s="26"/>
-      <c r="CS13" s="26"/>
-      <c r="CT13" s="26"/>
-      <c r="CU13" s="26"/>
-      <c r="CV13" s="26"/>
-      <c r="CW13" s="26"/>
-      <c r="CX13" s="26"/>
-      <c r="CY13" s="26"/>
-      <c r="CZ13" s="26"/>
-      <c r="DA13" s="26"/>
-      <c r="DB13" s="26"/>
-      <c r="DC13" s="26"/>
-      <c r="DD13" s="26"/>
-      <c r="DE13" s="26"/>
-      <c r="DF13" s="26"/>
-      <c r="DG13" s="26"/>
-      <c r="DH13" s="26"/>
-      <c r="DI13" s="26"/>
-      <c r="DJ13" s="26"/>
-      <c r="DK13" s="26"/>
-      <c r="DL13" s="26"/>
-      <c r="DM13" s="26"/>
-      <c r="DN13" s="26"/>
-      <c r="DO13" s="26"/>
-      <c r="DP13" s="26"/>
-      <c r="DQ13" s="26"/>
-      <c r="DR13" s="26"/>
-      <c r="DS13" s="26"/>
-      <c r="DT13" s="26"/>
-      <c r="DU13" s="26"/>
-      <c r="DV13" s="26"/>
-      <c r="DW13" s="26"/>
-      <c r="DX13" s="26"/>
-      <c r="DY13" s="26"/>
-      <c r="DZ13" s="26"/>
-      <c r="EA13" s="26"/>
-      <c r="EB13" s="26"/>
-      <c r="EC13" s="26"/>
-      <c r="ED13" s="26"/>
-      <c r="EE13" s="26"/>
-      <c r="EF13" s="26"/>
-      <c r="EG13" s="26"/>
-      <c r="EH13" s="26"/>
-      <c r="EI13" s="26"/>
-      <c r="EJ13" s="26"/>
-      <c r="EK13" s="26"/>
-      <c r="EL13" s="26"/>
-      <c r="EM13" s="26"/>
-      <c r="EN13" s="26"/>
-      <c r="EO13" s="26"/>
-      <c r="EP13" s="26"/>
-      <c r="EQ13" s="26"/>
-      <c r="ER13" s="26"/>
-      <c r="ES13" s="26"/>
-      <c r="ET13" s="26"/>
-      <c r="EU13" s="26"/>
-      <c r="EV13" s="26"/>
-      <c r="EW13" s="26"/>
-      <c r="EX13" s="26"/>
-      <c r="EY13" s="26"/>
-      <c r="EZ13" s="26"/>
-      <c r="FA13" s="26"/>
-      <c r="FB13" s="26"/>
-      <c r="FC13" s="26"/>
-      <c r="FD13" s="26"/>
-      <c r="FE13" s="26"/>
-      <c r="FF13" s="26"/>
-      <c r="FG13" s="26"/>
-      <c r="FH13" s="26"/>
-      <c r="FI13" s="26"/>
-      <c r="FJ13" s="26"/>
-      <c r="FK13" s="26"/>
-      <c r="FL13" s="26"/>
-      <c r="FM13" s="26"/>
-      <c r="FN13" s="26"/>
-      <c r="FO13" s="26"/>
-      <c r="FP13" s="26"/>
-      <c r="FQ13" s="26"/>
-      <c r="FR13" s="26"/>
-      <c r="FS13" s="26"/>
-      <c r="FT13" s="26"/>
-      <c r="FU13" s="26"/>
-      <c r="FV13" s="26"/>
-      <c r="FW13" s="26"/>
-      <c r="FX13" s="26"/>
-      <c r="FY13" s="26"/>
-      <c r="FZ13" s="26"/>
-      <c r="GA13" s="26"/>
-      <c r="GB13" s="26"/>
-      <c r="GC13" s="26"/>
-      <c r="GD13" s="26"/>
-      <c r="GE13" s="26"/>
-      <c r="GF13" s="26"/>
-      <c r="GG13" s="26"/>
-      <c r="GH13" s="26"/>
-      <c r="GI13" s="26"/>
-      <c r="GJ13" s="26"/>
-      <c r="GK13" s="26"/>
-      <c r="GL13" s="26"/>
-      <c r="GM13" s="26"/>
-      <c r="GN13" s="26"/>
-      <c r="GO13" s="26"/>
-      <c r="GP13" s="26"/>
-      <c r="GQ13" s="26"/>
-      <c r="GR13" s="26"/>
-      <c r="GS13" s="26"/>
-      <c r="GT13" s="26"/>
-      <c r="GU13" s="26"/>
-      <c r="GV13" s="26"/>
-      <c r="GW13" s="26"/>
-      <c r="GX13" s="26"/>
-      <c r="GY13" s="26"/>
-      <c r="GZ13" s="26"/>
-      <c r="HA13" s="26"/>
-      <c r="HB13" s="26"/>
-      <c r="HC13" s="26"/>
-      <c r="HD13" s="26"/>
-      <c r="HE13" s="26"/>
-      <c r="HF13" s="26"/>
-      <c r="HG13" s="26"/>
-      <c r="HH13" s="26"/>
-      <c r="HI13" s="26"/>
-      <c r="HJ13" s="26"/>
-      <c r="HK13" s="26"/>
-      <c r="HL13" s="26"/>
-      <c r="HM13" s="26"/>
-      <c r="HN13" s="26"/>
-      <c r="HO13" s="26"/>
-      <c r="HP13" s="26"/>
-      <c r="HQ13" s="26"/>
-      <c r="HR13" s="26"/>
-      <c r="HS13" s="26"/>
-      <c r="HT13" s="26"/>
-      <c r="HU13" s="26"/>
-      <c r="HV13" s="26"/>
-      <c r="HW13" s="26"/>
-      <c r="HX13" s="26"/>
-      <c r="HY13" s="26"/>
-      <c r="HZ13" s="26"/>
-      <c r="IA13" s="26"/>
-      <c r="IB13" s="26"/>
-      <c r="IC13" s="26"/>
-      <c r="ID13" s="26"/>
-      <c r="IE13" s="26"/>
-      <c r="IF13" s="26"/>
-      <c r="IG13" s="26"/>
-      <c r="IH13" s="26"/>
-      <c r="II13" s="26"/>
-      <c r="IJ13" s="26"/>
-      <c r="IK13" s="26"/>
-      <c r="IL13" s="26"/>
-      <c r="IM13" s="26"/>
-      <c r="IN13" s="26"/>
-      <c r="IO13" s="26"/>
-      <c r="IP13" s="26"/>
-      <c r="IQ13" s="26"/>
-      <c r="IR13" s="26"/>
-      <c r="IS13" s="26"/>
-      <c r="IT13" s="26"/>
-      <c r="IU13" s="26"/>
-      <c r="IV13" s="26"/>
-      <c r="IW13" s="26"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="27"/>
+      <c r="AA13" s="27"/>
+      <c r="AB13" s="27"/>
+      <c r="AC13" s="27"/>
+      <c r="AD13" s="27"/>
+      <c r="AE13" s="27"/>
+      <c r="AF13" s="27"/>
+      <c r="AG13" s="27"/>
+      <c r="AH13" s="27"/>
+      <c r="AI13" s="27"/>
+      <c r="AJ13" s="27"/>
+      <c r="AK13" s="27"/>
+      <c r="AL13" s="27"/>
+      <c r="AM13" s="27"/>
+      <c r="AN13" s="27"/>
+      <c r="AO13" s="27"/>
+      <c r="AP13" s="27"/>
+      <c r="AQ13" s="27"/>
+      <c r="AR13" s="27"/>
+      <c r="AS13" s="27"/>
+      <c r="AT13" s="27"/>
+      <c r="AU13" s="27"/>
+      <c r="AV13" s="27"/>
+      <c r="AW13" s="27"/>
+      <c r="AX13" s="27"/>
+      <c r="AY13" s="27"/>
+      <c r="AZ13" s="27"/>
+      <c r="BA13" s="27"/>
+      <c r="BB13" s="27"/>
+      <c r="BC13" s="27"/>
+      <c r="BD13" s="27"/>
+      <c r="BE13" s="27"/>
+      <c r="BF13" s="27"/>
+      <c r="BG13" s="27"/>
+      <c r="BH13" s="27"/>
+      <c r="BI13" s="27"/>
+      <c r="BJ13" s="27"/>
+      <c r="BK13" s="27"/>
+      <c r="BL13" s="27"/>
+      <c r="BM13" s="27"/>
+      <c r="BN13" s="27"/>
+      <c r="BO13" s="27"/>
+      <c r="BP13" s="27"/>
+      <c r="BQ13" s="27"/>
+      <c r="BR13" s="27"/>
+      <c r="BS13" s="27"/>
+      <c r="BT13" s="27"/>
+      <c r="BU13" s="27"/>
+      <c r="BV13" s="27"/>
+      <c r="BW13" s="27"/>
+      <c r="BX13" s="27"/>
+      <c r="BY13" s="27"/>
+      <c r="BZ13" s="27"/>
+      <c r="CA13" s="27"/>
+      <c r="CB13" s="27"/>
+      <c r="CC13" s="27"/>
+      <c r="CD13" s="27"/>
+      <c r="CE13" s="27"/>
+      <c r="CF13" s="27"/>
+      <c r="CG13" s="27"/>
+      <c r="CH13" s="27"/>
+      <c r="CI13" s="27"/>
+      <c r="CJ13" s="27"/>
+      <c r="CK13" s="27"/>
+      <c r="CL13" s="27"/>
+      <c r="CM13" s="27"/>
+      <c r="CN13" s="27"/>
+      <c r="CO13" s="27"/>
+      <c r="CP13" s="27"/>
+      <c r="CQ13" s="27"/>
+      <c r="CR13" s="27"/>
+      <c r="CS13" s="27"/>
+      <c r="CT13" s="27"/>
+      <c r="CU13" s="27"/>
+      <c r="CV13" s="27"/>
+      <c r="CW13" s="27"/>
+      <c r="CX13" s="27"/>
+      <c r="CY13" s="27"/>
+      <c r="CZ13" s="27"/>
+      <c r="DA13" s="27"/>
+      <c r="DB13" s="27"/>
+      <c r="DC13" s="27"/>
+      <c r="DD13" s="27"/>
+      <c r="DE13" s="27"/>
+      <c r="DF13" s="27"/>
+      <c r="DG13" s="27"/>
+      <c r="DH13" s="27"/>
+      <c r="DI13" s="27"/>
+      <c r="DJ13" s="27"/>
+      <c r="DK13" s="27"/>
+      <c r="DL13" s="27"/>
+      <c r="DM13" s="27"/>
+      <c r="DN13" s="27"/>
+      <c r="DO13" s="27"/>
+      <c r="DP13" s="27"/>
+      <c r="DQ13" s="27"/>
+      <c r="DR13" s="27"/>
+      <c r="DS13" s="27"/>
+      <c r="DT13" s="27"/>
+      <c r="DU13" s="27"/>
+      <c r="DV13" s="27"/>
+      <c r="DW13" s="27"/>
+      <c r="DX13" s="27"/>
+      <c r="DY13" s="27"/>
+      <c r="DZ13" s="27"/>
+      <c r="EA13" s="27"/>
+      <c r="EB13" s="27"/>
+      <c r="EC13" s="27"/>
+      <c r="ED13" s="27"/>
+      <c r="EE13" s="27"/>
+      <c r="EF13" s="27"/>
+      <c r="EG13" s="27"/>
+      <c r="EH13" s="27"/>
+      <c r="EI13" s="27"/>
+      <c r="EJ13" s="27"/>
+      <c r="EK13" s="27"/>
+      <c r="EL13" s="27"/>
+      <c r="EM13" s="27"/>
+      <c r="EN13" s="27"/>
+      <c r="EO13" s="27"/>
+      <c r="EP13" s="27"/>
+      <c r="EQ13" s="27"/>
+      <c r="ER13" s="27"/>
+      <c r="ES13" s="27"/>
+      <c r="ET13" s="27"/>
+      <c r="EU13" s="27"/>
+      <c r="EV13" s="27"/>
+      <c r="EW13" s="27"/>
+      <c r="EX13" s="27"/>
+      <c r="EY13" s="27"/>
+      <c r="EZ13" s="27"/>
+      <c r="FA13" s="27"/>
+      <c r="FB13" s="27"/>
+      <c r="FC13" s="27"/>
+      <c r="FD13" s="27"/>
+      <c r="FE13" s="27"/>
+      <c r="FF13" s="27"/>
+      <c r="FG13" s="27"/>
+      <c r="FH13" s="27"/>
+      <c r="FI13" s="27"/>
+      <c r="FJ13" s="27"/>
+      <c r="FK13" s="27"/>
+      <c r="FL13" s="27"/>
+      <c r="FM13" s="27"/>
+      <c r="FN13" s="27"/>
+      <c r="FO13" s="27"/>
+      <c r="FP13" s="27"/>
+      <c r="FQ13" s="27"/>
+      <c r="FR13" s="27"/>
+      <c r="FS13" s="27"/>
+      <c r="FT13" s="27"/>
+      <c r="FU13" s="27"/>
+      <c r="FV13" s="27"/>
+      <c r="FW13" s="27"/>
+      <c r="FX13" s="27"/>
+      <c r="FY13" s="27"/>
+      <c r="FZ13" s="27"/>
+      <c r="GA13" s="27"/>
+      <c r="GB13" s="27"/>
+      <c r="GC13" s="27"/>
+      <c r="GD13" s="27"/>
+      <c r="GE13" s="27"/>
+      <c r="GF13" s="27"/>
+      <c r="GG13" s="27"/>
+      <c r="GH13" s="27"/>
+      <c r="GI13" s="27"/>
+      <c r="GJ13" s="27"/>
+      <c r="GK13" s="27"/>
+      <c r="GL13" s="27"/>
+      <c r="GM13" s="27"/>
+      <c r="GN13" s="27"/>
+      <c r="GO13" s="27"/>
+      <c r="GP13" s="27"/>
+      <c r="GQ13" s="27"/>
+      <c r="GR13" s="27"/>
+      <c r="GS13" s="27"/>
+      <c r="GT13" s="27"/>
+      <c r="GU13" s="27"/>
+      <c r="GV13" s="27"/>
+      <c r="GW13" s="27"/>
+      <c r="GX13" s="27"/>
+      <c r="GY13" s="27"/>
+      <c r="GZ13" s="27"/>
+      <c r="HA13" s="27"/>
+      <c r="HB13" s="27"/>
+      <c r="HC13" s="27"/>
+      <c r="HD13" s="27"/>
+      <c r="HE13" s="27"/>
+      <c r="HF13" s="27"/>
+      <c r="HG13" s="27"/>
+      <c r="HH13" s="27"/>
+      <c r="HI13" s="27"/>
+      <c r="HJ13" s="27"/>
+      <c r="HK13" s="27"/>
+      <c r="HL13" s="27"/>
+      <c r="HM13" s="27"/>
+      <c r="HN13" s="27"/>
+      <c r="HO13" s="27"/>
+      <c r="HP13" s="27"/>
+      <c r="HQ13" s="27"/>
+      <c r="HR13" s="27"/>
+      <c r="HS13" s="27"/>
+      <c r="HT13" s="27"/>
+      <c r="HU13" s="27"/>
+      <c r="HV13" s="27"/>
+      <c r="HW13" s="27"/>
+      <c r="HX13" s="27"/>
+      <c r="HY13" s="27"/>
+      <c r="HZ13" s="27"/>
+      <c r="IA13" s="27"/>
+      <c r="IB13" s="27"/>
+      <c r="IC13" s="27"/>
+      <c r="ID13" s="27"/>
+      <c r="IE13" s="27"/>
+      <c r="IF13" s="27"/>
+      <c r="IG13" s="27"/>
+      <c r="IH13" s="27"/>
+      <c r="II13" s="27"/>
+      <c r="IJ13" s="27"/>
+      <c r="IK13" s="27"/>
+      <c r="IL13" s="27"/>
+      <c r="IM13" s="27"/>
+      <c r="IN13" s="27"/>
+      <c r="IO13" s="27"/>
+      <c r="IP13" s="27"/>
+      <c r="IQ13" s="27"/>
+      <c r="IR13" s="27"/>
+      <c r="IS13" s="27"/>
+      <c r="IT13" s="27"/>
+      <c r="IU13" s="27"/>
+      <c r="IV13" s="27"/>
+      <c r="IW13" s="27"/>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="21" t="n">
@@ -2670,252 +2674,252 @@
       <c r="K14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="U14" s="26"/>
-      <c r="V14" s="26"/>
-      <c r="W14" s="26"/>
-      <c r="X14" s="26"/>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="26"/>
-      <c r="AA14" s="26"/>
-      <c r="AB14" s="26"/>
-      <c r="AC14" s="26"/>
-      <c r="AD14" s="26"/>
-      <c r="AE14" s="26"/>
-      <c r="AF14" s="26"/>
-      <c r="AG14" s="26"/>
-      <c r="AH14" s="26"/>
-      <c r="AI14" s="26"/>
-      <c r="AJ14" s="26"/>
-      <c r="AK14" s="26"/>
-      <c r="AL14" s="26"/>
-      <c r="AM14" s="26"/>
-      <c r="AN14" s="26"/>
-      <c r="AO14" s="26"/>
-      <c r="AP14" s="26"/>
-      <c r="AQ14" s="26"/>
-      <c r="AR14" s="26"/>
-      <c r="AS14" s="26"/>
-      <c r="AT14" s="26"/>
-      <c r="AU14" s="26"/>
-      <c r="AV14" s="26"/>
-      <c r="AW14" s="26"/>
-      <c r="AX14" s="26"/>
-      <c r="AY14" s="26"/>
-      <c r="AZ14" s="26"/>
-      <c r="BA14" s="26"/>
-      <c r="BB14" s="26"/>
-      <c r="BC14" s="26"/>
-      <c r="BD14" s="26"/>
-      <c r="BE14" s="26"/>
-      <c r="BF14" s="26"/>
-      <c r="BG14" s="26"/>
-      <c r="BH14" s="26"/>
-      <c r="BI14" s="26"/>
-      <c r="BJ14" s="26"/>
-      <c r="BK14" s="26"/>
-      <c r="BL14" s="26"/>
-      <c r="BM14" s="26"/>
-      <c r="BN14" s="26"/>
-      <c r="BO14" s="26"/>
-      <c r="BP14" s="26"/>
-      <c r="BQ14" s="26"/>
-      <c r="BR14" s="26"/>
-      <c r="BS14" s="26"/>
-      <c r="BT14" s="26"/>
-      <c r="BU14" s="26"/>
-      <c r="BV14" s="26"/>
-      <c r="BW14" s="26"/>
-      <c r="BX14" s="26"/>
-      <c r="BY14" s="26"/>
-      <c r="BZ14" s="26"/>
-      <c r="CA14" s="26"/>
-      <c r="CB14" s="26"/>
-      <c r="CC14" s="26"/>
-      <c r="CD14" s="26"/>
-      <c r="CE14" s="26"/>
-      <c r="CF14" s="26"/>
-      <c r="CG14" s="26"/>
-      <c r="CH14" s="26"/>
-      <c r="CI14" s="26"/>
-      <c r="CJ14" s="26"/>
-      <c r="CK14" s="26"/>
-      <c r="CL14" s="26"/>
-      <c r="CM14" s="26"/>
-      <c r="CN14" s="26"/>
-      <c r="CO14" s="26"/>
-      <c r="CP14" s="26"/>
-      <c r="CQ14" s="26"/>
-      <c r="CR14" s="26"/>
-      <c r="CS14" s="26"/>
-      <c r="CT14" s="26"/>
-      <c r="CU14" s="26"/>
-      <c r="CV14" s="26"/>
-      <c r="CW14" s="26"/>
-      <c r="CX14" s="26"/>
-      <c r="CY14" s="26"/>
-      <c r="CZ14" s="26"/>
-      <c r="DA14" s="26"/>
-      <c r="DB14" s="26"/>
-      <c r="DC14" s="26"/>
-      <c r="DD14" s="26"/>
-      <c r="DE14" s="26"/>
-      <c r="DF14" s="26"/>
-      <c r="DG14" s="26"/>
-      <c r="DH14" s="26"/>
-      <c r="DI14" s="26"/>
-      <c r="DJ14" s="26"/>
-      <c r="DK14" s="26"/>
-      <c r="DL14" s="26"/>
-      <c r="DM14" s="26"/>
-      <c r="DN14" s="26"/>
-      <c r="DO14" s="26"/>
-      <c r="DP14" s="26"/>
-      <c r="DQ14" s="26"/>
-      <c r="DR14" s="26"/>
-      <c r="DS14" s="26"/>
-      <c r="DT14" s="26"/>
-      <c r="DU14" s="26"/>
-      <c r="DV14" s="26"/>
-      <c r="DW14" s="26"/>
-      <c r="DX14" s="26"/>
-      <c r="DY14" s="26"/>
-      <c r="DZ14" s="26"/>
-      <c r="EA14" s="26"/>
-      <c r="EB14" s="26"/>
-      <c r="EC14" s="26"/>
-      <c r="ED14" s="26"/>
-      <c r="EE14" s="26"/>
-      <c r="EF14" s="26"/>
-      <c r="EG14" s="26"/>
-      <c r="EH14" s="26"/>
-      <c r="EI14" s="26"/>
-      <c r="EJ14" s="26"/>
-      <c r="EK14" s="26"/>
-      <c r="EL14" s="26"/>
-      <c r="EM14" s="26"/>
-      <c r="EN14" s="26"/>
-      <c r="EO14" s="26"/>
-      <c r="EP14" s="26"/>
-      <c r="EQ14" s="26"/>
-      <c r="ER14" s="26"/>
-      <c r="ES14" s="26"/>
-      <c r="ET14" s="26"/>
-      <c r="EU14" s="26"/>
-      <c r="EV14" s="26"/>
-      <c r="EW14" s="26"/>
-      <c r="EX14" s="26"/>
-      <c r="EY14" s="26"/>
-      <c r="EZ14" s="26"/>
-      <c r="FA14" s="26"/>
-      <c r="FB14" s="26"/>
-      <c r="FC14" s="26"/>
-      <c r="FD14" s="26"/>
-      <c r="FE14" s="26"/>
-      <c r="FF14" s="26"/>
-      <c r="FG14" s="26"/>
-      <c r="FH14" s="26"/>
-      <c r="FI14" s="26"/>
-      <c r="FJ14" s="26"/>
-      <c r="FK14" s="26"/>
-      <c r="FL14" s="26"/>
-      <c r="FM14" s="26"/>
-      <c r="FN14" s="26"/>
-      <c r="FO14" s="26"/>
-      <c r="FP14" s="26"/>
-      <c r="FQ14" s="26"/>
-      <c r="FR14" s="26"/>
-      <c r="FS14" s="26"/>
-      <c r="FT14" s="26"/>
-      <c r="FU14" s="26"/>
-      <c r="FV14" s="26"/>
-      <c r="FW14" s="26"/>
-      <c r="FX14" s="26"/>
-      <c r="FY14" s="26"/>
-      <c r="FZ14" s="26"/>
-      <c r="GA14" s="26"/>
-      <c r="GB14" s="26"/>
-      <c r="GC14" s="26"/>
-      <c r="GD14" s="26"/>
-      <c r="GE14" s="26"/>
-      <c r="GF14" s="26"/>
-      <c r="GG14" s="26"/>
-      <c r="GH14" s="26"/>
-      <c r="GI14" s="26"/>
-      <c r="GJ14" s="26"/>
-      <c r="GK14" s="26"/>
-      <c r="GL14" s="26"/>
-      <c r="GM14" s="26"/>
-      <c r="GN14" s="26"/>
-      <c r="GO14" s="26"/>
-      <c r="GP14" s="26"/>
-      <c r="GQ14" s="26"/>
-      <c r="GR14" s="26"/>
-      <c r="GS14" s="26"/>
-      <c r="GT14" s="26"/>
-      <c r="GU14" s="26"/>
-      <c r="GV14" s="26"/>
-      <c r="GW14" s="26"/>
-      <c r="GX14" s="26"/>
-      <c r="GY14" s="26"/>
-      <c r="GZ14" s="26"/>
-      <c r="HA14" s="26"/>
-      <c r="HB14" s="26"/>
-      <c r="HC14" s="26"/>
-      <c r="HD14" s="26"/>
-      <c r="HE14" s="26"/>
-      <c r="HF14" s="26"/>
-      <c r="HG14" s="26"/>
-      <c r="HH14" s="26"/>
-      <c r="HI14" s="26"/>
-      <c r="HJ14" s="26"/>
-      <c r="HK14" s="26"/>
-      <c r="HL14" s="26"/>
-      <c r="HM14" s="26"/>
-      <c r="HN14" s="26"/>
-      <c r="HO14" s="26"/>
-      <c r="HP14" s="26"/>
-      <c r="HQ14" s="26"/>
-      <c r="HR14" s="26"/>
-      <c r="HS14" s="26"/>
-      <c r="HT14" s="26"/>
-      <c r="HU14" s="26"/>
-      <c r="HV14" s="26"/>
-      <c r="HW14" s="26"/>
-      <c r="HX14" s="26"/>
-      <c r="HY14" s="26"/>
-      <c r="HZ14" s="26"/>
-      <c r="IA14" s="26"/>
-      <c r="IB14" s="26"/>
-      <c r="IC14" s="26"/>
-      <c r="ID14" s="26"/>
-      <c r="IE14" s="26"/>
-      <c r="IF14" s="26"/>
-      <c r="IG14" s="26"/>
-      <c r="IH14" s="26"/>
-      <c r="II14" s="26"/>
-      <c r="IJ14" s="26"/>
-      <c r="IK14" s="26"/>
-      <c r="IL14" s="26"/>
-      <c r="IM14" s="26"/>
-      <c r="IN14" s="26"/>
-      <c r="IO14" s="26"/>
-      <c r="IP14" s="26"/>
-      <c r="IQ14" s="26"/>
-      <c r="IR14" s="26"/>
-      <c r="IS14" s="26"/>
-      <c r="IT14" s="26"/>
-      <c r="IU14" s="26"/>
-      <c r="IV14" s="26"/>
-      <c r="IW14" s="26"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+      <c r="AA14" s="27"/>
+      <c r="AB14" s="27"/>
+      <c r="AC14" s="27"/>
+      <c r="AD14" s="27"/>
+      <c r="AE14" s="27"/>
+      <c r="AF14" s="27"/>
+      <c r="AG14" s="27"/>
+      <c r="AH14" s="27"/>
+      <c r="AI14" s="27"/>
+      <c r="AJ14" s="27"/>
+      <c r="AK14" s="27"/>
+      <c r="AL14" s="27"/>
+      <c r="AM14" s="27"/>
+      <c r="AN14" s="27"/>
+      <c r="AO14" s="27"/>
+      <c r="AP14" s="27"/>
+      <c r="AQ14" s="27"/>
+      <c r="AR14" s="27"/>
+      <c r="AS14" s="27"/>
+      <c r="AT14" s="27"/>
+      <c r="AU14" s="27"/>
+      <c r="AV14" s="27"/>
+      <c r="AW14" s="27"/>
+      <c r="AX14" s="27"/>
+      <c r="AY14" s="27"/>
+      <c r="AZ14" s="27"/>
+      <c r="BA14" s="27"/>
+      <c r="BB14" s="27"/>
+      <c r="BC14" s="27"/>
+      <c r="BD14" s="27"/>
+      <c r="BE14" s="27"/>
+      <c r="BF14" s="27"/>
+      <c r="BG14" s="27"/>
+      <c r="BH14" s="27"/>
+      <c r="BI14" s="27"/>
+      <c r="BJ14" s="27"/>
+      <c r="BK14" s="27"/>
+      <c r="BL14" s="27"/>
+      <c r="BM14" s="27"/>
+      <c r="BN14" s="27"/>
+      <c r="BO14" s="27"/>
+      <c r="BP14" s="27"/>
+      <c r="BQ14" s="27"/>
+      <c r="BR14" s="27"/>
+      <c r="BS14" s="27"/>
+      <c r="BT14" s="27"/>
+      <c r="BU14" s="27"/>
+      <c r="BV14" s="27"/>
+      <c r="BW14" s="27"/>
+      <c r="BX14" s="27"/>
+      <c r="BY14" s="27"/>
+      <c r="BZ14" s="27"/>
+      <c r="CA14" s="27"/>
+      <c r="CB14" s="27"/>
+      <c r="CC14" s="27"/>
+      <c r="CD14" s="27"/>
+      <c r="CE14" s="27"/>
+      <c r="CF14" s="27"/>
+      <c r="CG14" s="27"/>
+      <c r="CH14" s="27"/>
+      <c r="CI14" s="27"/>
+      <c r="CJ14" s="27"/>
+      <c r="CK14" s="27"/>
+      <c r="CL14" s="27"/>
+      <c r="CM14" s="27"/>
+      <c r="CN14" s="27"/>
+      <c r="CO14" s="27"/>
+      <c r="CP14" s="27"/>
+      <c r="CQ14" s="27"/>
+      <c r="CR14" s="27"/>
+      <c r="CS14" s="27"/>
+      <c r="CT14" s="27"/>
+      <c r="CU14" s="27"/>
+      <c r="CV14" s="27"/>
+      <c r="CW14" s="27"/>
+      <c r="CX14" s="27"/>
+      <c r="CY14" s="27"/>
+      <c r="CZ14" s="27"/>
+      <c r="DA14" s="27"/>
+      <c r="DB14" s="27"/>
+      <c r="DC14" s="27"/>
+      <c r="DD14" s="27"/>
+      <c r="DE14" s="27"/>
+      <c r="DF14" s="27"/>
+      <c r="DG14" s="27"/>
+      <c r="DH14" s="27"/>
+      <c r="DI14" s="27"/>
+      <c r="DJ14" s="27"/>
+      <c r="DK14" s="27"/>
+      <c r="DL14" s="27"/>
+      <c r="DM14" s="27"/>
+      <c r="DN14" s="27"/>
+      <c r="DO14" s="27"/>
+      <c r="DP14" s="27"/>
+      <c r="DQ14" s="27"/>
+      <c r="DR14" s="27"/>
+      <c r="DS14" s="27"/>
+      <c r="DT14" s="27"/>
+      <c r="DU14" s="27"/>
+      <c r="DV14" s="27"/>
+      <c r="DW14" s="27"/>
+      <c r="DX14" s="27"/>
+      <c r="DY14" s="27"/>
+      <c r="DZ14" s="27"/>
+      <c r="EA14" s="27"/>
+      <c r="EB14" s="27"/>
+      <c r="EC14" s="27"/>
+      <c r="ED14" s="27"/>
+      <c r="EE14" s="27"/>
+      <c r="EF14" s="27"/>
+      <c r="EG14" s="27"/>
+      <c r="EH14" s="27"/>
+      <c r="EI14" s="27"/>
+      <c r="EJ14" s="27"/>
+      <c r="EK14" s="27"/>
+      <c r="EL14" s="27"/>
+      <c r="EM14" s="27"/>
+      <c r="EN14" s="27"/>
+      <c r="EO14" s="27"/>
+      <c r="EP14" s="27"/>
+      <c r="EQ14" s="27"/>
+      <c r="ER14" s="27"/>
+      <c r="ES14" s="27"/>
+      <c r="ET14" s="27"/>
+      <c r="EU14" s="27"/>
+      <c r="EV14" s="27"/>
+      <c r="EW14" s="27"/>
+      <c r="EX14" s="27"/>
+      <c r="EY14" s="27"/>
+      <c r="EZ14" s="27"/>
+      <c r="FA14" s="27"/>
+      <c r="FB14" s="27"/>
+      <c r="FC14" s="27"/>
+      <c r="FD14" s="27"/>
+      <c r="FE14" s="27"/>
+      <c r="FF14" s="27"/>
+      <c r="FG14" s="27"/>
+      <c r="FH14" s="27"/>
+      <c r="FI14" s="27"/>
+      <c r="FJ14" s="27"/>
+      <c r="FK14" s="27"/>
+      <c r="FL14" s="27"/>
+      <c r="FM14" s="27"/>
+      <c r="FN14" s="27"/>
+      <c r="FO14" s="27"/>
+      <c r="FP14" s="27"/>
+      <c r="FQ14" s="27"/>
+      <c r="FR14" s="27"/>
+      <c r="FS14" s="27"/>
+      <c r="FT14" s="27"/>
+      <c r="FU14" s="27"/>
+      <c r="FV14" s="27"/>
+      <c r="FW14" s="27"/>
+      <c r="FX14" s="27"/>
+      <c r="FY14" s="27"/>
+      <c r="FZ14" s="27"/>
+      <c r="GA14" s="27"/>
+      <c r="GB14" s="27"/>
+      <c r="GC14" s="27"/>
+      <c r="GD14" s="27"/>
+      <c r="GE14" s="27"/>
+      <c r="GF14" s="27"/>
+      <c r="GG14" s="27"/>
+      <c r="GH14" s="27"/>
+      <c r="GI14" s="27"/>
+      <c r="GJ14" s="27"/>
+      <c r="GK14" s="27"/>
+      <c r="GL14" s="27"/>
+      <c r="GM14" s="27"/>
+      <c r="GN14" s="27"/>
+      <c r="GO14" s="27"/>
+      <c r="GP14" s="27"/>
+      <c r="GQ14" s="27"/>
+      <c r="GR14" s="27"/>
+      <c r="GS14" s="27"/>
+      <c r="GT14" s="27"/>
+      <c r="GU14" s="27"/>
+      <c r="GV14" s="27"/>
+      <c r="GW14" s="27"/>
+      <c r="GX14" s="27"/>
+      <c r="GY14" s="27"/>
+      <c r="GZ14" s="27"/>
+      <c r="HA14" s="27"/>
+      <c r="HB14" s="27"/>
+      <c r="HC14" s="27"/>
+      <c r="HD14" s="27"/>
+      <c r="HE14" s="27"/>
+      <c r="HF14" s="27"/>
+      <c r="HG14" s="27"/>
+      <c r="HH14" s="27"/>
+      <c r="HI14" s="27"/>
+      <c r="HJ14" s="27"/>
+      <c r="HK14" s="27"/>
+      <c r="HL14" s="27"/>
+      <c r="HM14" s="27"/>
+      <c r="HN14" s="27"/>
+      <c r="HO14" s="27"/>
+      <c r="HP14" s="27"/>
+      <c r="HQ14" s="27"/>
+      <c r="HR14" s="27"/>
+      <c r="HS14" s="27"/>
+      <c r="HT14" s="27"/>
+      <c r="HU14" s="27"/>
+      <c r="HV14" s="27"/>
+      <c r="HW14" s="27"/>
+      <c r="HX14" s="27"/>
+      <c r="HY14" s="27"/>
+      <c r="HZ14" s="27"/>
+      <c r="IA14" s="27"/>
+      <c r="IB14" s="27"/>
+      <c r="IC14" s="27"/>
+      <c r="ID14" s="27"/>
+      <c r="IE14" s="27"/>
+      <c r="IF14" s="27"/>
+      <c r="IG14" s="27"/>
+      <c r="IH14" s="27"/>
+      <c r="II14" s="27"/>
+      <c r="IJ14" s="27"/>
+      <c r="IK14" s="27"/>
+      <c r="IL14" s="27"/>
+      <c r="IM14" s="27"/>
+      <c r="IN14" s="27"/>
+      <c r="IO14" s="27"/>
+      <c r="IP14" s="27"/>
+      <c r="IQ14" s="27"/>
+      <c r="IR14" s="27"/>
+      <c r="IS14" s="27"/>
+      <c r="IT14" s="27"/>
+      <c r="IU14" s="27"/>
+      <c r="IV14" s="27"/>
+      <c r="IW14" s="27"/>
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="21" t="n">
@@ -2924,7 +2928,7 @@
       <c r="B15" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="28" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="22"/>
@@ -2934,7 +2938,7 @@
       <c r="F15" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="28" t="s">
         <v>54</v>
       </c>
       <c r="H15" s="21"/>
@@ -2945,262 +2949,262 @@
       <c r="K15" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="26"/>
-      <c r="S15" s="26"/>
-      <c r="T15" s="26"/>
-      <c r="U15" s="26"/>
-      <c r="V15" s="26"/>
-      <c r="W15" s="26"/>
-      <c r="X15" s="26"/>
-      <c r="Y15" s="26"/>
-      <c r="Z15" s="26"/>
-      <c r="AA15" s="26"/>
-      <c r="AB15" s="26"/>
-      <c r="AC15" s="26"/>
-      <c r="AD15" s="26"/>
-      <c r="AE15" s="26"/>
-      <c r="AF15" s="26"/>
-      <c r="AG15" s="26"/>
-      <c r="AH15" s="26"/>
-      <c r="AI15" s="26"/>
-      <c r="AJ15" s="26"/>
-      <c r="AK15" s="26"/>
-      <c r="AL15" s="26"/>
-      <c r="AM15" s="26"/>
-      <c r="AN15" s="26"/>
-      <c r="AO15" s="26"/>
-      <c r="AP15" s="26"/>
-      <c r="AQ15" s="26"/>
-      <c r="AR15" s="26"/>
-      <c r="AS15" s="26"/>
-      <c r="AT15" s="26"/>
-      <c r="AU15" s="26"/>
-      <c r="AV15" s="26"/>
-      <c r="AW15" s="26"/>
-      <c r="AX15" s="26"/>
-      <c r="AY15" s="26"/>
-      <c r="AZ15" s="26"/>
-      <c r="BA15" s="26"/>
-      <c r="BB15" s="26"/>
-      <c r="BC15" s="26"/>
-      <c r="BD15" s="26"/>
-      <c r="BE15" s="26"/>
-      <c r="BF15" s="26"/>
-      <c r="BG15" s="26"/>
-      <c r="BH15" s="26"/>
-      <c r="BI15" s="26"/>
-      <c r="BJ15" s="26"/>
-      <c r="BK15" s="26"/>
-      <c r="BL15" s="26"/>
-      <c r="BM15" s="26"/>
-      <c r="BN15" s="26"/>
-      <c r="BO15" s="26"/>
-      <c r="BP15" s="26"/>
-      <c r="BQ15" s="26"/>
-      <c r="BR15" s="26"/>
-      <c r="BS15" s="26"/>
-      <c r="BT15" s="26"/>
-      <c r="BU15" s="26"/>
-      <c r="BV15" s="26"/>
-      <c r="BW15" s="26"/>
-      <c r="BX15" s="26"/>
-      <c r="BY15" s="26"/>
-      <c r="BZ15" s="26"/>
-      <c r="CA15" s="26"/>
-      <c r="CB15" s="26"/>
-      <c r="CC15" s="26"/>
-      <c r="CD15" s="26"/>
-      <c r="CE15" s="26"/>
-      <c r="CF15" s="26"/>
-      <c r="CG15" s="26"/>
-      <c r="CH15" s="26"/>
-      <c r="CI15" s="26"/>
-      <c r="CJ15" s="26"/>
-      <c r="CK15" s="26"/>
-      <c r="CL15" s="26"/>
-      <c r="CM15" s="26"/>
-      <c r="CN15" s="26"/>
-      <c r="CO15" s="26"/>
-      <c r="CP15" s="26"/>
-      <c r="CQ15" s="26"/>
-      <c r="CR15" s="26"/>
-      <c r="CS15" s="26"/>
-      <c r="CT15" s="26"/>
-      <c r="CU15" s="26"/>
-      <c r="CV15" s="26"/>
-      <c r="CW15" s="26"/>
-      <c r="CX15" s="26"/>
-      <c r="CY15" s="26"/>
-      <c r="CZ15" s="26"/>
-      <c r="DA15" s="26"/>
-      <c r="DB15" s="26"/>
-      <c r="DC15" s="26"/>
-      <c r="DD15" s="26"/>
-      <c r="DE15" s="26"/>
-      <c r="DF15" s="26"/>
-      <c r="DG15" s="26"/>
-      <c r="DH15" s="26"/>
-      <c r="DI15" s="26"/>
-      <c r="DJ15" s="26"/>
-      <c r="DK15" s="26"/>
-      <c r="DL15" s="26"/>
-      <c r="DM15" s="26"/>
-      <c r="DN15" s="26"/>
-      <c r="DO15" s="26"/>
-      <c r="DP15" s="26"/>
-      <c r="DQ15" s="26"/>
-      <c r="DR15" s="26"/>
-      <c r="DS15" s="26"/>
-      <c r="DT15" s="26"/>
-      <c r="DU15" s="26"/>
-      <c r="DV15" s="26"/>
-      <c r="DW15" s="26"/>
-      <c r="DX15" s="26"/>
-      <c r="DY15" s="26"/>
-      <c r="DZ15" s="26"/>
-      <c r="EA15" s="26"/>
-      <c r="EB15" s="26"/>
-      <c r="EC15" s="26"/>
-      <c r="ED15" s="26"/>
-      <c r="EE15" s="26"/>
-      <c r="EF15" s="26"/>
-      <c r="EG15" s="26"/>
-      <c r="EH15" s="26"/>
-      <c r="EI15" s="26"/>
-      <c r="EJ15" s="26"/>
-      <c r="EK15" s="26"/>
-      <c r="EL15" s="26"/>
-      <c r="EM15" s="26"/>
-      <c r="EN15" s="26"/>
-      <c r="EO15" s="26"/>
-      <c r="EP15" s="26"/>
-      <c r="EQ15" s="26"/>
-      <c r="ER15" s="26"/>
-      <c r="ES15" s="26"/>
-      <c r="ET15" s="26"/>
-      <c r="EU15" s="26"/>
-      <c r="EV15" s="26"/>
-      <c r="EW15" s="26"/>
-      <c r="EX15" s="26"/>
-      <c r="EY15" s="26"/>
-      <c r="EZ15" s="26"/>
-      <c r="FA15" s="26"/>
-      <c r="FB15" s="26"/>
-      <c r="FC15" s="26"/>
-      <c r="FD15" s="26"/>
-      <c r="FE15" s="26"/>
-      <c r="FF15" s="26"/>
-      <c r="FG15" s="26"/>
-      <c r="FH15" s="26"/>
-      <c r="FI15" s="26"/>
-      <c r="FJ15" s="26"/>
-      <c r="FK15" s="26"/>
-      <c r="FL15" s="26"/>
-      <c r="FM15" s="26"/>
-      <c r="FN15" s="26"/>
-      <c r="FO15" s="26"/>
-      <c r="FP15" s="26"/>
-      <c r="FQ15" s="26"/>
-      <c r="FR15" s="26"/>
-      <c r="FS15" s="26"/>
-      <c r="FT15" s="26"/>
-      <c r="FU15" s="26"/>
-      <c r="FV15" s="26"/>
-      <c r="FW15" s="26"/>
-      <c r="FX15" s="26"/>
-      <c r="FY15" s="26"/>
-      <c r="FZ15" s="26"/>
-      <c r="GA15" s="26"/>
-      <c r="GB15" s="26"/>
-      <c r="GC15" s="26"/>
-      <c r="GD15" s="26"/>
-      <c r="GE15" s="26"/>
-      <c r="GF15" s="26"/>
-      <c r="GG15" s="26"/>
-      <c r="GH15" s="26"/>
-      <c r="GI15" s="26"/>
-      <c r="GJ15" s="26"/>
-      <c r="GK15" s="26"/>
-      <c r="GL15" s="26"/>
-      <c r="GM15" s="26"/>
-      <c r="GN15" s="26"/>
-      <c r="GO15" s="26"/>
-      <c r="GP15" s="26"/>
-      <c r="GQ15" s="26"/>
-      <c r="GR15" s="26"/>
-      <c r="GS15" s="26"/>
-      <c r="GT15" s="26"/>
-      <c r="GU15" s="26"/>
-      <c r="GV15" s="26"/>
-      <c r="GW15" s="26"/>
-      <c r="GX15" s="26"/>
-      <c r="GY15" s="26"/>
-      <c r="GZ15" s="26"/>
-      <c r="HA15" s="26"/>
-      <c r="HB15" s="26"/>
-      <c r="HC15" s="26"/>
-      <c r="HD15" s="26"/>
-      <c r="HE15" s="26"/>
-      <c r="HF15" s="26"/>
-      <c r="HG15" s="26"/>
-      <c r="HH15" s="26"/>
-      <c r="HI15" s="26"/>
-      <c r="HJ15" s="26"/>
-      <c r="HK15" s="26"/>
-      <c r="HL15" s="26"/>
-      <c r="HM15" s="26"/>
-      <c r="HN15" s="26"/>
-      <c r="HO15" s="26"/>
-      <c r="HP15" s="26"/>
-      <c r="HQ15" s="26"/>
-      <c r="HR15" s="26"/>
-      <c r="HS15" s="26"/>
-      <c r="HT15" s="26"/>
-      <c r="HU15" s="26"/>
-      <c r="HV15" s="26"/>
-      <c r="HW15" s="26"/>
-      <c r="HX15" s="26"/>
-      <c r="HY15" s="26"/>
-      <c r="HZ15" s="26"/>
-      <c r="IA15" s="26"/>
-      <c r="IB15" s="26"/>
-      <c r="IC15" s="26"/>
-      <c r="ID15" s="26"/>
-      <c r="IE15" s="26"/>
-      <c r="IF15" s="26"/>
-      <c r="IG15" s="26"/>
-      <c r="IH15" s="26"/>
-      <c r="II15" s="26"/>
-      <c r="IJ15" s="26"/>
-      <c r="IK15" s="26"/>
-      <c r="IL15" s="26"/>
-      <c r="IM15" s="26"/>
-      <c r="IN15" s="26"/>
-      <c r="IO15" s="26"/>
-      <c r="IP15" s="26"/>
-      <c r="IQ15" s="26"/>
-      <c r="IR15" s="26"/>
-      <c r="IS15" s="26"/>
-      <c r="IT15" s="26"/>
-      <c r="IU15" s="26"/>
-      <c r="IV15" s="26"/>
-      <c r="IW15" s="26"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="27"/>
+      <c r="Y15" s="27"/>
+      <c r="Z15" s="27"/>
+      <c r="AA15" s="27"/>
+      <c r="AB15" s="27"/>
+      <c r="AC15" s="27"/>
+      <c r="AD15" s="27"/>
+      <c r="AE15" s="27"/>
+      <c r="AF15" s="27"/>
+      <c r="AG15" s="27"/>
+      <c r="AH15" s="27"/>
+      <c r="AI15" s="27"/>
+      <c r="AJ15" s="27"/>
+      <c r="AK15" s="27"/>
+      <c r="AL15" s="27"/>
+      <c r="AM15" s="27"/>
+      <c r="AN15" s="27"/>
+      <c r="AO15" s="27"/>
+      <c r="AP15" s="27"/>
+      <c r="AQ15" s="27"/>
+      <c r="AR15" s="27"/>
+      <c r="AS15" s="27"/>
+      <c r="AT15" s="27"/>
+      <c r="AU15" s="27"/>
+      <c r="AV15" s="27"/>
+      <c r="AW15" s="27"/>
+      <c r="AX15" s="27"/>
+      <c r="AY15" s="27"/>
+      <c r="AZ15" s="27"/>
+      <c r="BA15" s="27"/>
+      <c r="BB15" s="27"/>
+      <c r="BC15" s="27"/>
+      <c r="BD15" s="27"/>
+      <c r="BE15" s="27"/>
+      <c r="BF15" s="27"/>
+      <c r="BG15" s="27"/>
+      <c r="BH15" s="27"/>
+      <c r="BI15" s="27"/>
+      <c r="BJ15" s="27"/>
+      <c r="BK15" s="27"/>
+      <c r="BL15" s="27"/>
+      <c r="BM15" s="27"/>
+      <c r="BN15" s="27"/>
+      <c r="BO15" s="27"/>
+      <c r="BP15" s="27"/>
+      <c r="BQ15" s="27"/>
+      <c r="BR15" s="27"/>
+      <c r="BS15" s="27"/>
+      <c r="BT15" s="27"/>
+      <c r="BU15" s="27"/>
+      <c r="BV15" s="27"/>
+      <c r="BW15" s="27"/>
+      <c r="BX15" s="27"/>
+      <c r="BY15" s="27"/>
+      <c r="BZ15" s="27"/>
+      <c r="CA15" s="27"/>
+      <c r="CB15" s="27"/>
+      <c r="CC15" s="27"/>
+      <c r="CD15" s="27"/>
+      <c r="CE15" s="27"/>
+      <c r="CF15" s="27"/>
+      <c r="CG15" s="27"/>
+      <c r="CH15" s="27"/>
+      <c r="CI15" s="27"/>
+      <c r="CJ15" s="27"/>
+      <c r="CK15" s="27"/>
+      <c r="CL15" s="27"/>
+      <c r="CM15" s="27"/>
+      <c r="CN15" s="27"/>
+      <c r="CO15" s="27"/>
+      <c r="CP15" s="27"/>
+      <c r="CQ15" s="27"/>
+      <c r="CR15" s="27"/>
+      <c r="CS15" s="27"/>
+      <c r="CT15" s="27"/>
+      <c r="CU15" s="27"/>
+      <c r="CV15" s="27"/>
+      <c r="CW15" s="27"/>
+      <c r="CX15" s="27"/>
+      <c r="CY15" s="27"/>
+      <c r="CZ15" s="27"/>
+      <c r="DA15" s="27"/>
+      <c r="DB15" s="27"/>
+      <c r="DC15" s="27"/>
+      <c r="DD15" s="27"/>
+      <c r="DE15" s="27"/>
+      <c r="DF15" s="27"/>
+      <c r="DG15" s="27"/>
+      <c r="DH15" s="27"/>
+      <c r="DI15" s="27"/>
+      <c r="DJ15" s="27"/>
+      <c r="DK15" s="27"/>
+      <c r="DL15" s="27"/>
+      <c r="DM15" s="27"/>
+      <c r="DN15" s="27"/>
+      <c r="DO15" s="27"/>
+      <c r="DP15" s="27"/>
+      <c r="DQ15" s="27"/>
+      <c r="DR15" s="27"/>
+      <c r="DS15" s="27"/>
+      <c r="DT15" s="27"/>
+      <c r="DU15" s="27"/>
+      <c r="DV15" s="27"/>
+      <c r="DW15" s="27"/>
+      <c r="DX15" s="27"/>
+      <c r="DY15" s="27"/>
+      <c r="DZ15" s="27"/>
+      <c r="EA15" s="27"/>
+      <c r="EB15" s="27"/>
+      <c r="EC15" s="27"/>
+      <c r="ED15" s="27"/>
+      <c r="EE15" s="27"/>
+      <c r="EF15" s="27"/>
+      <c r="EG15" s="27"/>
+      <c r="EH15" s="27"/>
+      <c r="EI15" s="27"/>
+      <c r="EJ15" s="27"/>
+      <c r="EK15" s="27"/>
+      <c r="EL15" s="27"/>
+      <c r="EM15" s="27"/>
+      <c r="EN15" s="27"/>
+      <c r="EO15" s="27"/>
+      <c r="EP15" s="27"/>
+      <c r="EQ15" s="27"/>
+      <c r="ER15" s="27"/>
+      <c r="ES15" s="27"/>
+      <c r="ET15" s="27"/>
+      <c r="EU15" s="27"/>
+      <c r="EV15" s="27"/>
+      <c r="EW15" s="27"/>
+      <c r="EX15" s="27"/>
+      <c r="EY15" s="27"/>
+      <c r="EZ15" s="27"/>
+      <c r="FA15" s="27"/>
+      <c r="FB15" s="27"/>
+      <c r="FC15" s="27"/>
+      <c r="FD15" s="27"/>
+      <c r="FE15" s="27"/>
+      <c r="FF15" s="27"/>
+      <c r="FG15" s="27"/>
+      <c r="FH15" s="27"/>
+      <c r="FI15" s="27"/>
+      <c r="FJ15" s="27"/>
+      <c r="FK15" s="27"/>
+      <c r="FL15" s="27"/>
+      <c r="FM15" s="27"/>
+      <c r="FN15" s="27"/>
+      <c r="FO15" s="27"/>
+      <c r="FP15" s="27"/>
+      <c r="FQ15" s="27"/>
+      <c r="FR15" s="27"/>
+      <c r="FS15" s="27"/>
+      <c r="FT15" s="27"/>
+      <c r="FU15" s="27"/>
+      <c r="FV15" s="27"/>
+      <c r="FW15" s="27"/>
+      <c r="FX15" s="27"/>
+      <c r="FY15" s="27"/>
+      <c r="FZ15" s="27"/>
+      <c r="GA15" s="27"/>
+      <c r="GB15" s="27"/>
+      <c r="GC15" s="27"/>
+      <c r="GD15" s="27"/>
+      <c r="GE15" s="27"/>
+      <c r="GF15" s="27"/>
+      <c r="GG15" s="27"/>
+      <c r="GH15" s="27"/>
+      <c r="GI15" s="27"/>
+      <c r="GJ15" s="27"/>
+      <c r="GK15" s="27"/>
+      <c r="GL15" s="27"/>
+      <c r="GM15" s="27"/>
+      <c r="GN15" s="27"/>
+      <c r="GO15" s="27"/>
+      <c r="GP15" s="27"/>
+      <c r="GQ15" s="27"/>
+      <c r="GR15" s="27"/>
+      <c r="GS15" s="27"/>
+      <c r="GT15" s="27"/>
+      <c r="GU15" s="27"/>
+      <c r="GV15" s="27"/>
+      <c r="GW15" s="27"/>
+      <c r="GX15" s="27"/>
+      <c r="GY15" s="27"/>
+      <c r="GZ15" s="27"/>
+      <c r="HA15" s="27"/>
+      <c r="HB15" s="27"/>
+      <c r="HC15" s="27"/>
+      <c r="HD15" s="27"/>
+      <c r="HE15" s="27"/>
+      <c r="HF15" s="27"/>
+      <c r="HG15" s="27"/>
+      <c r="HH15" s="27"/>
+      <c r="HI15" s="27"/>
+      <c r="HJ15" s="27"/>
+      <c r="HK15" s="27"/>
+      <c r="HL15" s="27"/>
+      <c r="HM15" s="27"/>
+      <c r="HN15" s="27"/>
+      <c r="HO15" s="27"/>
+      <c r="HP15" s="27"/>
+      <c r="HQ15" s="27"/>
+      <c r="HR15" s="27"/>
+      <c r="HS15" s="27"/>
+      <c r="HT15" s="27"/>
+      <c r="HU15" s="27"/>
+      <c r="HV15" s="27"/>
+      <c r="HW15" s="27"/>
+      <c r="HX15" s="27"/>
+      <c r="HY15" s="27"/>
+      <c r="HZ15" s="27"/>
+      <c r="IA15" s="27"/>
+      <c r="IB15" s="27"/>
+      <c r="IC15" s="27"/>
+      <c r="ID15" s="27"/>
+      <c r="IE15" s="27"/>
+      <c r="IF15" s="27"/>
+      <c r="IG15" s="27"/>
+      <c r="IH15" s="27"/>
+      <c r="II15" s="27"/>
+      <c r="IJ15" s="27"/>
+      <c r="IK15" s="27"/>
+      <c r="IL15" s="27"/>
+      <c r="IM15" s="27"/>
+      <c r="IN15" s="27"/>
+      <c r="IO15" s="27"/>
+      <c r="IP15" s="27"/>
+      <c r="IQ15" s="27"/>
+      <c r="IR15" s="27"/>
+      <c r="IS15" s="27"/>
+      <c r="IT15" s="27"/>
+      <c r="IU15" s="27"/>
+      <c r="IV15" s="27"/>
+      <c r="IW15" s="27"/>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="30"/>
+      <c r="E16" s="31"/>
       <c r="F16" s="1"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="31"/>
+      <c r="H16" s="32"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -3209,9 +3213,9 @@
       <c r="A17" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="D17" s="33"/>
-      <c r="G17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="D17" s="34"/>
+      <c r="G17" s="34"/>
     </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>